<commit_message>
Changed Balanced IO card de-emphasis circuit in AM RoW variant to match pre-emphasis changes in previous commit
</commit_message>
<xml_diff>
--- a/balio/BoM am row.xlsx
+++ b/balio/BoM am row.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tom\Documents\Electronics\amtx\Audio\amproc\balio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796ED4A6-F4AE-4DC3-B97D-339CA014CF67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3585D662-109E-4EE6-B93D-80392B5AC5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -247,48 +247,12 @@
     <t>R8 R16</t>
   </si>
   <si>
-    <t>2n7</t>
-  </si>
-  <si>
-    <t>20k</t>
-  </si>
-  <si>
-    <t>7k5</t>
-  </si>
-  <si>
     <t>Radial box W7.2mm T2.5mm S5mm</t>
   </si>
   <si>
-    <t>2.7nF 100V 10% film</t>
-  </si>
-  <si>
     <t>Kemet</t>
   </si>
   <si>
-    <t>R82EC1270AA50K</t>
-  </si>
-  <si>
-    <t>80-R82EC1270AA50K</t>
-  </si>
-  <si>
-    <t>20k 0.6W 1% metal film</t>
-  </si>
-  <si>
-    <t>MCMF006FF2002A50</t>
-  </si>
-  <si>
-    <t>2301788</t>
-  </si>
-  <si>
-    <t>7.5k 0.6W 1% metal film</t>
-  </si>
-  <si>
-    <t>MCMF006FF7501A50</t>
-  </si>
-  <si>
-    <t>2401777</t>
-  </si>
-  <si>
     <t>NC3FAAH2</t>
   </si>
   <si>
@@ -308,6 +272,42 @@
   </si>
   <si>
     <t>ESK107M025AE3AA</t>
+  </si>
+  <si>
+    <t>8k2</t>
+  </si>
+  <si>
+    <t>5k1</t>
+  </si>
+  <si>
+    <t>5n6</t>
+  </si>
+  <si>
+    <t>5.6nF 63V 5% film</t>
+  </si>
+  <si>
+    <t>MMK5562J63J01L16.5TA18</t>
+  </si>
+  <si>
+    <t>80-MMK5562J63J01TA18</t>
+  </si>
+  <si>
+    <t>8.2k 0.6W 1% metal film</t>
+  </si>
+  <si>
+    <t>MCMF006FF8201A50</t>
+  </si>
+  <si>
+    <t>2401778</t>
+  </si>
+  <si>
+    <t>5.1k 0.6W 1% metal film</t>
+  </si>
+  <si>
+    <t>MCMF006FF5101A50</t>
+  </si>
+  <si>
+    <t>2401773</t>
   </si>
 </sst>
 </file>
@@ -1299,55 +1299,55 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" t="s">
         <v>75</v>
       </c>
-      <c r="D4" t="s">
-        <v>78</v>
-      </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G4" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="H4" t="s">
         <v>62</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J4" s="6">
-        <v>0.20599999999999999</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="K4" s="7">
         <f t="shared" si="0"/>
-        <v>0.41199999999999998</v>
+        <v>0.45800000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G5" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="H5" t="s">
         <v>29</v>
@@ -1371,7 +1371,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
@@ -1380,13 +1380,13 @@
         <v>47</v>
       </c>
       <c r="G6" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="H6" t="s">
         <v>29</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="J6" s="6">
         <v>0.93899999999999995</v>
@@ -1611,32 +1611,32 @@
         <v>2</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D13" t="s">
         <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="F13" t="s">
         <v>53</v>
       </c>
       <c r="G13" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="H13" t="s">
         <v>29</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="J13" s="6">
-        <v>0.03</v>
+        <v>2.8400000000000002E-2</v>
       </c>
       <c r="K13" s="7">
         <f t="shared" si="0"/>
-        <v>0.06</v>
+        <v>5.6800000000000003E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
@@ -1647,32 +1647,32 @@
         <v>2</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D14" t="s">
         <v>51</v>
       </c>
       <c r="E14" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="F14" t="s">
         <v>53</v>
       </c>
       <c r="G14" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="H14" t="s">
         <v>29</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="J14" s="6">
-        <v>2.86E-2</v>
+        <v>3.7900000000000003E-2</v>
       </c>
       <c r="K14" s="7">
         <f t="shared" si="0"/>
-        <v>5.7200000000000001E-2</v>
+        <v>7.5800000000000006E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.4">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="K18" s="7">
         <f>SUM(K2:K16)</f>
-        <v>25.201199999999996</v>
+        <v>25.262599999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>